<commit_message>
Add a safer CSV download option for patient data templates
Add a new CSV file for patient data templates and update the UI to offer a CSV download option for patient data, alongside the existing XLSX option, to address potential virus detection issues with the XLSX file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ee57d091-bb9c-492e-ac6f-1dbf58feeaa6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f4188f4d-b026-473e-945a-5a0b13d4deff/ee57d091-bb9c-492e-ac6f-1dbf58feeaa6/QGN3wAf
</commit_message>
<xml_diff>
--- a/public/modelo_pacientes.xlsx
+++ b/public/modelo_pacientes.xlsx
@@ -401,21 +401,6 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -460,43 +445,43 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>João da Silva</v>
+        <v>Maria Silva</v>
       </c>
       <c r="B2" t="str">
-        <v>QR 123 Conjunto 10 Casa 15</v>
+        <v>QR 100 Conjunto 5 Casa 20</v>
       </c>
       <c r="C2" t="str">
         <v>72000-000</v>
       </c>
       <c r="D2" t="str">
-        <v>João</v>
+        <v/>
       </c>
       <c r="E2" t="str">
-        <v>Maria da Silva</v>
+        <v/>
       </c>
       <c r="F2" t="str">
-        <v>15/03/1985</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>39</v>
+        <v/>
       </c>
       <c r="H2" t="str">
-        <v>123.456.789-00</v>
+        <v/>
       </c>
       <c r="I2" t="str">
-        <v>(61) 99999-9999</v>
+        <v>(61) 98888-8888</v>
       </c>
       <c r="J2" t="str">
-        <v>Cisgênero</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>Pardo</v>
+        <v/>
       </c>
       <c r="L2" t="str">
-        <v>Hipertensão, Diabetes</v>
+        <v/>
       </c>
       <c r="M2" t="str">
-        <v>01/10/2025</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>